<commit_message>
Updates/new spreads for carbon
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/Drift-ion.xlsx
+++ b/21-Spreads4Tests/Drift-ion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/Library/CloudStorage/Box-Box/CubMac-Box/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/2047436751938/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EFF88B-046A-AA4E-96BD-BF60919484CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{77EFF88B-046A-AA4E-96BD-BF60919484CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{351409D8-658E-2649-A9BD-1FF2C7B9E30E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -625,6 +625,16 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,20 +653,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,7 +970,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="H27" sqref="H27:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,26 +984,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
-      <c r="H1" s="33" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="39"/>
+      <c r="H1" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="35"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" spans="1:10" ht="20" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
       <c r="D2" s="21"/>
       <c r="E2" s="20" t="s">
         <v>26</v>
@@ -1125,11 +1121,11 @@
       <c r="C7" s="6"/>
       <c r="D7" s="30"/>
       <c r="E7" s="31"/>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="34"/>
-      <c r="J7" s="35"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="39"/>
     </row>
     <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
@@ -1140,17 +1136,17 @@
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="27"/>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="33" t="s">
         <v>30</v>
       </c>
       <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.2">
       <c r="D9" s="1"/>
-      <c r="H9" s="41" t="s">
+      <c r="H9" s="34" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="19">
@@ -1161,13 +1157,13 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="1"/>
-      <c r="H10" s="42" t="s">
+      <c r="H10" s="35" t="s">
         <v>31</v>
       </c>
       <c r="I10" s="18">
@@ -1259,7 +1255,7 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20">
         <v>0</v>
       </c>
       <c r="G20" s="19">
@@ -1281,7 +1277,7 @@
         <f>E3</f>
         <v>1.5</v>
       </c>
-      <c r="F21" s="43">
+      <c r="F21">
         <v>0</v>
       </c>
       <c r="G21" s="19">
@@ -1301,7 +1297,7 @@
       <c r="E22" s="9">
         <v>1</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F22">
         <v>0</v>
       </c>
       <c r="G22" s="19">
@@ -1326,7 +1322,7 @@
       <c r="F23" s="17">
         <v>1</v>
       </c>
-      <c r="G23" s="44">
+      <c r="G23" s="36">
         <f>E3/B6^2</f>
         <v>418.6803352764465</v>
       </c>

</xml_diff>